<commit_message>
Custom List and Fluid Layouts
</commit_message>
<xml_diff>
--- a/2024FEB_B3_Daily_Class.xlsx
+++ b/2024FEB_B3_Daily_Class.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>S.N.</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Pseudo classes</t>
+  </si>
+  <si>
+    <t>Custom List and Fluid Layout</t>
   </si>
 </sst>
 </file>
@@ -1434,7 +1437,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
       <c r="A79" s="7">
         <v>78</v>
       </c>
@@ -1443,7 +1446,7 @@
       </c>
       <c r="C79" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
       <c r="A80" s="7">
         <v>79</v>
       </c>
@@ -1452,7 +1455,7 @@
       </c>
       <c r="C80" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
       <c r="A81" s="7">
         <v>80</v>
       </c>
@@ -1461,7 +1464,7 @@
       </c>
       <c r="C81" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
       <c r="A82" s="7">
         <v>81</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
       <c r="A83" s="7">
         <v>82</v>
       </c>
@@ -1481,7 +1484,7 @@
       </c>
       <c r="C83" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
       <c r="A84" s="7">
         <v>83</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
       <c r="A85" s="7">
         <v>84</v>
       </c>
@@ -1503,16 +1506,18 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="7">
         <v>85</v>
       </c>
       <c r="B86" s="8">
         <v>45417</v>
       </c>
-      <c r="C86" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+      <c r="C86" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
       <c r="A87" s="7">
         <v>86</v>
       </c>
@@ -1521,7 +1526,7 @@
       </c>
       <c r="C87" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="7">
         <v>87</v>
       </c>
@@ -1530,7 +1535,7 @@
       </c>
       <c r="C88" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
       <c r="A89" s="7">
         <v>88</v>
       </c>
@@ -1539,7 +1544,7 @@
       </c>
       <c r="C89" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
       <c r="A90" s="7">
         <v>89</v>
       </c>
@@ -1548,7 +1553,7 @@
       </c>
       <c r="C90" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
       <c r="A91" s="7">
         <v>90</v>
       </c>
@@ -1557,7 +1562,7 @@
       </c>
       <c r="C91" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
       <c r="A92" s="7">
         <v>91</v>
       </c>
@@ -1566,7 +1571,7 @@
       </c>
       <c r="C92" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
       <c r="A93" s="7">
         <v>92</v>
       </c>
@@ -1575,7 +1580,7 @@
       </c>
       <c r="C93" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
       <c r="A94" s="7">
         <v>93</v>
       </c>
@@ -1584,7 +1589,7 @@
       </c>
       <c r="C94" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
       <c r="A95" s="7">
         <v>94</v>
       </c>
@@ -1593,7 +1598,7 @@
       </c>
       <c r="C95" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
       <c r="A96" s="7">
         <v>95</v>
       </c>
@@ -1602,7 +1607,7 @@
       </c>
       <c r="C96" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
       <c r="A97" s="7">
         <v>96</v>
       </c>
@@ -1611,7 +1616,7 @@
       </c>
       <c r="C97" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
       <c r="A98" s="7">
         <v>97</v>
       </c>
@@ -1620,7 +1625,7 @@
       </c>
       <c r="C98" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
       <c r="A99" s="7">
         <v>98</v>
       </c>
@@ -1629,7 +1634,7 @@
       </c>
       <c r="C99" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
       <c r="A100" s="7">
         <v>99</v>
       </c>
@@ -1638,7 +1643,7 @@
       </c>
       <c r="C100" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
       <c r="A101" s="7">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Getting started with PHP
</commit_message>
<xml_diff>
--- a/2024FEB_B3_Daily_Class.xlsx
+++ b/2024FEB_B3_Daily_Class.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
     <t>S.N.</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>Custom List and Fluid Layout</t>
+  </si>
+  <si>
+    <t>Fluid Layout</t>
+  </si>
+  <si>
+    <t>Media Query</t>
+  </si>
+  <si>
+    <t>Getting Started with PHP</t>
   </si>
 </sst>
 </file>
@@ -1524,7 +1533,9 @@
       <c r="B87" s="8">
         <v>45418</v>
       </c>
-      <c r="C87" s="9"/>
+      <c r="C87" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="7">
@@ -1533,7 +1544,9 @@
       <c r="B88" s="8">
         <v>45419</v>
       </c>
-      <c r="C88" s="9"/>
+      <c r="C88" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
       <c r="A89" s="7">
@@ -1542,7 +1555,9 @@
       <c r="B89" s="8">
         <v>45420</v>
       </c>
-      <c r="C89" s="9"/>
+      <c r="C89" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
       <c r="A90" s="7">
@@ -1551,7 +1566,9 @@
       <c r="B90" s="8">
         <v>45421</v>
       </c>
-      <c r="C90" s="9"/>
+      <c r="C90" s="9" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
       <c r="A91" s="7">
@@ -1652,7 +1669,7 @@
       </c>
       <c r="C101" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
       <c r="A102" s="7">
         <v>101</v>
       </c>
@@ -1661,7 +1678,7 @@
       </c>
       <c r="C102" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5">
       <c r="A103" s="7">
         <v>102</v>
       </c>
@@ -1670,7 +1687,7 @@
       </c>
       <c r="C103" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
       <c r="A104" s="7">
         <v>103</v>
       </c>
@@ -1679,7 +1696,7 @@
       </c>
       <c r="C104" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5">
       <c r="A105" s="7">
         <v>104</v>
       </c>
@@ -1688,7 +1705,7 @@
       </c>
       <c r="C105" s="9"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="20.25">
       <c r="A106" s="7">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
Control statements in PHP
</commit_message>
<xml_diff>
--- a/2024FEB_B3_Daily_Class.xlsx
+++ b/2024FEB_B3_Daily_Class.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t>S.N.</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>Getting Started with PHP</t>
+  </si>
+  <si>
+    <t>Getting started with PHP</t>
+  </si>
+  <si>
+    <t>Control statements in PHP</t>
   </si>
 </sst>
 </file>
@@ -1577,7 +1583,9 @@
       <c r="B91" s="8">
         <v>45422</v>
       </c>
-      <c r="C91" s="9"/>
+      <c r="C91" s="9" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
       <c r="A92" s="7">
@@ -1586,7 +1594,9 @@
       <c r="B92" s="8">
         <v>45423</v>
       </c>
-      <c r="C92" s="9"/>
+      <c r="C92" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
       <c r="A93" s="7">
@@ -1595,7 +1605,9 @@
       <c r="B93" s="8">
         <v>45424</v>
       </c>
-      <c r="C93" s="9"/>
+      <c r="C93" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
       <c r="A94" s="7">

</xml_diff>

<commit_message>
date time text and nums
</commit_message>
<xml_diff>
--- a/2024FEB_B3_Daily_Class.xlsx
+++ b/2024FEB_B3_Daily_Class.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
   <si>
     <t>S.N.</t>
   </si>
@@ -170,6 +170,19 @@
   </si>
   <si>
     <t>Associative and Multidimensional array</t>
+  </si>
+  <si>
+    <t>Multidimensional array and working with date and time</t>
+  </si>
+  <si>
+    <t>No class due to Micro Teaching Evaluation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No class due to Micro Teaching Evaluation
+</t>
+  </si>
+  <si>
+    <t>Date time, Text and nums</t>
   </si>
 </sst>
 </file>
@@ -1658,7 +1671,9 @@
       <c r="B97" s="8">
         <v>45428</v>
       </c>
-      <c r="C97" s="9"/>
+      <c r="C97" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
       <c r="A98" s="7">
@@ -1667,7 +1682,9 @@
       <c r="B98" s="8">
         <v>45429</v>
       </c>
-      <c r="C98" s="9"/>
+      <c r="C98" s="9" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
       <c r="A99" s="7">
@@ -1676,7 +1693,9 @@
       <c r="B99" s="8">
         <v>45430</v>
       </c>
-      <c r="C99" s="9"/>
+      <c r="C99" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
       <c r="A100" s="7">
@@ -1685,7 +1704,9 @@
       <c r="B100" s="8">
         <v>45431</v>
       </c>
-      <c r="C100" s="9"/>
+      <c r="C100" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
       <c r="A101" s="7">
@@ -1694,7 +1715,9 @@
       <c r="B101" s="8">
         <v>45432</v>
       </c>
-      <c r="C101" s="9"/>
+      <c r="C101" s="9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
       <c r="A102" s="7">

</xml_diff>